<commit_message>
feat: Finish some buttons call back declartion
</commit_message>
<xml_diff>
--- a/hw01_calc/TouchGFX/assets/texts/texts.xlsx
+++ b/hw01_calc/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="87">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t xml:space="preserve">result :p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sleepy</t>
   </si>
 </sst>
 </file>
@@ -2053,7 +2056,7 @@
         <v>44</v>
       </c>
       <c r="F22" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new widget: txt_debug, function unimplemented
Refactor: Change names of some widgets.

For reviewing changes, just diff TouchGFX/hw01_calc.touchgfx.
Others are auto generated by touchGFX.
</commit_message>
<xml_diff>
--- a/hw01_calc/TouchGFX/assets/texts/texts.xlsx
+++ b/hw01_calc/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2024" uniqueCount="95">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -276,6 +276,30 @@
   </si>
   <si>
     <t xml:space="preserve">sleepy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res_txt_debug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clicked: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clicked</t>
   </si>
 </sst>
 </file>
@@ -2059,6 +2083,24 @@
         <v>86</v>
       </c>
     </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
misc: Machine genrated codes from next commit
Since they are machine genrated, you don't need to review on this commit.
</commit_message>
<xml_diff>
--- a/hw01_calc/TouchGFX/assets/texts/texts.xlsx
+++ b/hw01_calc/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2024" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3158" uniqueCount="103">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -300,6 +300,30 @@
   </si>
   <si>
     <t xml:space="preserve">clicked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdefg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;result&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB-ALIGNMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -1759,6 +1783,9 @@
       <c r="F3" t="s">
         <v>36</v>
       </c>
+      <c r="G3" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" t="s">
@@ -2068,7 +2095,7 @@
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
         <v>38</v>
@@ -2080,27 +2107,80 @@
         <v>44</v>
       </c>
       <c r="F22" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
         <v>38</v>
       </c>
       <c r="D23" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
         <v>43</v>
       </c>
-      <c r="E23" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" t="s">
+        <v>100</v>
+      </c>
+      <c r="G24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="24"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Fix #1 displaying ? with some characters by setting wildcards
It's because I forgot to read the documents carefully.
TouchGFX generates only used characters to glyphs(bitmap). If you want to change the display text at runtime, you should force generates the glyphs of characters that you are going to display.
By doing this, open touchGFX project, go to Texts->Typographics->Wildcard Characters, add your characters here.
For more information: https://support.touchgfx.com/docs/development/ui-development/designer-user-guide/texts-view

*Note that file changes in this commit are all machine generated, so no need for code review.
*The wildcards here are different from f4f1f19, textAreaWithOneWildcard.
</commit_message>
<xml_diff>
--- a/hw01_calc/TouchGFX/assets/texts/texts.xlsx
+++ b/hw01_calc/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3158" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4353" uniqueCount="108">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -324,6 +324,21 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-z,A-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">" "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"+-*/. "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"+-*/."</t>
   </si>
 </sst>
 </file>
@@ -1565,9 +1580,13 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
+      <c r="G4" t="s">
+        <v>106</v>
+      </c>
       <c r="H4"/>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>103</v>
+      </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
@@ -1586,23 +1605,6 @@
       </c>
     </row>
     <row r="5" spans="2:16">
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5">
-        <v>40</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5"/>
-      <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="L5" s="7" t="s">
@@ -1620,23 +1622,6 @@
       <c r="P5" s="10"/>
     </row>
     <row r="6" spans="2:16">
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6"/>
-      <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
       <c r="L6" s="7" t="s">

</xml_diff>